<commit_message>
Inclusão da documentação de projeto
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lluca\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\são paulo tech school\2-Semestre\Pesquisa e Inovação\Tech_Health\secundarios\Documentos-grupo9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D87BA8B4-907A-4972-ACBA-32929C1397DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7618EFC8-229B-4B23-8EE1-CB89BCEE5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{095729ED-C60A-4FD3-9E98-E33A118FD078}"/>
   </bookViews>
@@ -201,13 +201,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +525,7 @@
   <dimension ref="C4:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,181 +539,181 @@
   </cols>
   <sheetData>
     <row r="4" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -727,6 +727,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100892A8A68E1C8AD4BB8607B0553D331B3" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74b2e3f3a56bee18fe3a2a59198b03e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a087c55-5f08-466c-910b-e029fd4269fe" xmlns:ns4="e2ca784f-4dc5-42e9-9734-389708ce15cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9979899fd4933bb41c74c0c74c549ba" ns3:_="" ns4:_="">
     <xsd:import namespace="7a087c55-5f08-466c-910b-e029fd4269fe"/>
@@ -897,15 +906,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -913,6 +913,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E604F19-924C-49D9-AB44-F9078FCCA316}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45F2D608-0561-467D-AD28-6F6122EB1535}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -931,14 +939,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E604F19-924C-49D9-AB44-F9078FCCA316}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD2D642-0A1D-44D6-8B56-C6D07CE173B3}">
   <ds:schemaRefs>

</xml_diff>